<commit_message>
Adiciona circuito quadro elétrico
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lesc\Desktop\inversor-documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8A4C5F-8F6D-4496-A184-3BE922CB8F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0318CA2-5C99-4D1A-8943-17553E25D595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{56CD8641-A580-4AF9-9D2A-88D91AD13176}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
-  <si>
-    <t>Cronograma</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
   <si>
     <t>Etapa</t>
   </si>
@@ -70,6 +67,33 @@
   </si>
   <si>
     <t>8. Revisão do Trabalho</t>
+  </si>
+  <si>
+    <t>2. Implementação do código no ESP32</t>
+  </si>
+  <si>
+    <t>3. Teste da implementação do código</t>
+  </si>
+  <si>
+    <t>4. Implementação do Aplicativo</t>
+  </si>
+  <si>
+    <t>5. Teste do aplicativo</t>
+  </si>
+  <si>
+    <t>7. Verificar se o projeto atende aos requisitos</t>
+  </si>
+  <si>
+    <t>1. Implementação de Hardware (Inclui criação do circuito de comunicação Serial)</t>
+  </si>
+  <si>
+    <t>8. Revisar projeto caso não atenda os requisitos</t>
+  </si>
+  <si>
+    <t>Cronograma do TCC</t>
+  </si>
+  <si>
+    <t>Cronograma da Implementação</t>
   </si>
 </sst>
 </file>
@@ -151,19 +175,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,138 +509,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42C879F-0617-464A-A72F-B7B63E3B5910}">
-  <dimension ref="F3:J12"/>
+  <dimension ref="F3:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F15" sqref="F15:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="40.85546875" customWidth="1"/>
+    <col min="6" max="6" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="6:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="3" t="s">
+    </row>
+    <row r="5" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="6:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="1"/>
+      <c r="G18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F15:J15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>